<commit_message>
updated test files and parameters
</commit_message>
<xml_diff>
--- a/data/test_data/2022_04_22_NEG_RSL3DAAvsCtrl_mz-d_identification_test_output.xlsx
+++ b/data/test_data/2022_04_22_NEG_RSL3DAAvsCtrl_mz-d_identification_test_output.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/678a94a76f9ec8c6/Documents/School - Graduate/ms code test files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_0FEA7100686B5EEF5E448AF12F38434B4BE96E0D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B4063F1-3F75-4567-AD98-CC456E04BD23}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="3150" yWindow="300" windowWidth="16260" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Identifications" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="52">
   <si>
     <t>mz</t>
   </si>
@@ -65,15 +71,6 @@
     <t>meas_mz_rt_ccs</t>
   </si>
   <si>
-    <t>pred_mz_rt</t>
-  </si>
-  <si>
-    <t>pred_mz</t>
-  </si>
-  <si>
-    <t>pred_mz_ccs</t>
-  </si>
-  <si>
     <t>PI(40:7)_[M+CH3COO]-</t>
   </si>
   <si>
@@ -110,27 +107,12 @@
     <t>PI(37:4)_[M-H]-</t>
   </si>
   <si>
-    <t>PI(o36:8)_[M+Cl]-</t>
-  </si>
-  <si>
-    <t>PI(p36:12)_[M+HCOO]-</t>
-  </si>
-  <si>
-    <t>PIP3(17:2)_[M+Cl]-</t>
-  </si>
-  <si>
     <t>PC(38:5)_[M+CH3COO]-</t>
   </si>
   <si>
     <t>PA(44:6)_[M+CH3COO]-</t>
   </si>
   <si>
-    <t>PC(42:10)_[M-H]-</t>
-  </si>
-  <si>
-    <t>PC(38:12)_[M+CH3COO]-</t>
-  </si>
-  <si>
     <t>PC(38:6)_[M+HCOO]-</t>
   </si>
   <si>
@@ -167,70 +149,25 @@
     <t>PI(p36:3)_[M+Cl]-</t>
   </si>
   <si>
-    <t>PI(34:6)_[M+HCOO]-</t>
-  </si>
-  <si>
-    <t>PIP(p29:3)_[M+HCOO]-</t>
-  </si>
-  <si>
     <t>PA(45:6)_[M+HCOO]-</t>
   </si>
   <si>
-    <t>PS(38:1)_[M+Cl]-</t>
-  </si>
-  <si>
-    <t>PS(42:11)_[M-H]-</t>
-  </si>
-  <si>
     <t>PI(38:7)_[M-H]-</t>
   </si>
   <si>
-    <t>PI(33:6)_[M+CH3COO]-</t>
-  </si>
-  <si>
-    <t>PIP(p28:3)_[M+CH3COO]-</t>
-  </si>
-  <si>
     <t>PA(o47:8)_[M+Cl]-</t>
   </si>
   <si>
-    <t>PE(45:10)_[M-H]-</t>
-  </si>
-  <si>
-    <t>PE(41:12)_[M+CH3COO]-</t>
-  </si>
-  <si>
     <t>PS(44:4)_[M-H]-</t>
   </si>
   <si>
-    <t>PI(p36:7)_[M+Cl]-</t>
-  </si>
-  <si>
-    <t>PIP(o29:4)_[M+HCOO]-</t>
-  </si>
-  <si>
-    <t>PS(p40:7)_[M+Cl]-</t>
-  </si>
-  <si>
     <t>PC(15:0/20:3)_[M+CH3COO]-</t>
   </si>
   <si>
     <t>PC(p43:6)_[M+Cl]-</t>
   </si>
   <si>
-    <t>PIP(o28:4)_[M+CH3COO]-</t>
-  </si>
-  <si>
-    <t>PC(39:12)_[M+HCOO]-</t>
-  </si>
-  <si>
     <t>PE(40:6)_[M+CH3COO]-</t>
-  </si>
-  <si>
-    <t>PS(o40:8)_[M+Cl]-</t>
-  </si>
-  <si>
-    <t>PE(42:12)_[M+HCOO]-</t>
   </si>
   <si>
     <t>PC(15:0/22:6)_[M+CH3COO]-</t>
@@ -245,8 +182,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +246,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -355,7 +300,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -387,9 +332,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -421,6 +384,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -596,14 +577,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -638,59 +621,59 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>967.5522655</v>
+        <v>967.55226549999998</v>
       </c>
       <c r="C2">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D2">
-        <v>312.5144217</v>
+        <v>312.51442170000001</v>
       </c>
       <c r="E2">
-        <v>934.6214866</v>
+        <v>934.62148660000003</v>
       </c>
       <c r="F2">
-        <v>1094.73544</v>
+        <v>1094.7354399999999</v>
       </c>
       <c r="G2">
-        <v>954.8222422</v>
+        <v>954.82224220000001</v>
       </c>
       <c r="H2">
         <v>927.0848565</v>
       </c>
       <c r="I2">
-        <v>6602.049053</v>
+        <v>6602.0490529999997</v>
       </c>
       <c r="J2">
-        <v>6641.527883</v>
+        <v>6641.5278829999997</v>
       </c>
       <c r="K2">
-        <v>7256.793762</v>
+        <v>7256.7937620000002</v>
       </c>
       <c r="L2">
-        <v>7581.589184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>7581.5891840000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>967.5520752</v>
+        <v>967.55207519999999</v>
       </c>
       <c r="C3">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D3">
-        <v>312.4874341</v>
+        <v>312.48743409999997</v>
       </c>
       <c r="E3">
-        <v>275.6045971</v>
+        <v>275.60459709999998</v>
       </c>
       <c r="F3">
         <v>325.3869894</v>
@@ -699,22 +682,22 @@
         <v>257.9792104</v>
       </c>
       <c r="H3">
-        <v>221.7834394</v>
+        <v>221.78343939999999</v>
       </c>
       <c r="I3">
-        <v>5145.522914</v>
+        <v>5145.5229140000001</v>
       </c>
       <c r="J3">
-        <v>5188.327403</v>
+        <v>5188.3274030000002</v>
       </c>
       <c r="K3">
-        <v>5715.824612</v>
+        <v>5715.8246120000003</v>
       </c>
       <c r="L3">
-        <v>6050.710903</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>6050.7109030000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -722,364 +705,364 @@
         <v>965.5342114</v>
       </c>
       <c r="C4">
-        <v>1.018716667</v>
+        <v>1.0187166670000001</v>
       </c>
       <c r="D4">
-        <v>308.3125788</v>
+        <v>308.31257879999998</v>
       </c>
       <c r="E4">
-        <v>447.0995745</v>
+        <v>447.09957450000002</v>
       </c>
       <c r="F4">
-        <v>568.0319381</v>
+        <v>568.03193810000005</v>
       </c>
       <c r="G4">
-        <v>469.3748422</v>
+        <v>469.37484219999999</v>
       </c>
       <c r="H4">
-        <v>449.8296461</v>
+        <v>449.82964609999999</v>
       </c>
       <c r="I4">
         <v>2290.23477</v>
       </c>
       <c r="J4">
-        <v>2399.960504</v>
+        <v>2399.9605040000001</v>
       </c>
       <c r="K4">
         <v>2324.603286</v>
       </c>
       <c r="L4">
-        <v>2844.648241</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>2844.6482409999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>965.5318508</v>
+        <v>965.53185080000003</v>
       </c>
       <c r="C5">
-        <v>1.018716667</v>
+        <v>1.0187166670000001</v>
       </c>
       <c r="D5">
-        <v>308.3393262</v>
+        <v>308.33932620000002</v>
       </c>
       <c r="E5">
-        <v>1810.925229</v>
+        <v>1810.9252289999999</v>
       </c>
       <c r="F5">
-        <v>2170.762825</v>
+        <v>2170.7628249999998</v>
       </c>
       <c r="G5">
-        <v>2037.408507</v>
+        <v>2037.4085070000001</v>
       </c>
       <c r="H5">
         <v>1907.618416</v>
       </c>
       <c r="I5">
-        <v>4358.48966</v>
+        <v>4358.4896600000002</v>
       </c>
       <c r="J5">
-        <v>4484.772675</v>
+        <v>4484.7726750000002</v>
       </c>
       <c r="K5">
-        <v>4198.418976</v>
+        <v>4198.4189759999999</v>
       </c>
       <c r="L5">
-        <v>5014.240737</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>5014.2407370000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>938.5822902</v>
+        <v>938.58229019999999</v>
       </c>
       <c r="C6">
-        <v>3.312083333</v>
+        <v>3.3120833329999999</v>
       </c>
       <c r="D6">
-        <v>301.4248499</v>
+        <v>301.42484990000003</v>
       </c>
       <c r="E6">
-        <v>942.7501483</v>
+        <v>942.75014829999998</v>
       </c>
       <c r="F6">
         <v>1360.577998</v>
       </c>
       <c r="G6">
-        <v>1146.238086</v>
+        <v>1146.2380860000001</v>
       </c>
       <c r="H6">
-        <v>956.8825965</v>
+        <v>956.88259649999998</v>
       </c>
       <c r="I6">
-        <v>2574.424026</v>
+        <v>2574.4240260000001</v>
       </c>
       <c r="J6">
-        <v>2488.655095</v>
+        <v>2488.6550950000001</v>
       </c>
       <c r="K6">
-        <v>2684.108101</v>
+        <v>2684.1081009999998</v>
       </c>
       <c r="L6">
         <v>3130.453943</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>938.5804534</v>
+        <v>938.58045340000001</v>
       </c>
       <c r="C7">
-        <v>3.312083333</v>
+        <v>3.3120833329999999</v>
       </c>
       <c r="D7">
         <v>302.8109753</v>
       </c>
       <c r="E7">
-        <v>32.9625708</v>
+        <v>32.962570800000002</v>
       </c>
       <c r="F7">
-        <v>45.51309597</v>
+        <v>45.513095970000002</v>
       </c>
       <c r="G7">
         <v>49.66554884</v>
       </c>
       <c r="H7">
-        <v>37.82272856</v>
+        <v>37.822728560000002</v>
       </c>
       <c r="I7">
         <v>1868.771356</v>
       </c>
       <c r="J7">
-        <v>1875.234317</v>
+        <v>1875.2343169999999</v>
       </c>
       <c r="K7">
-        <v>2083.74659</v>
+        <v>2083.7465900000002</v>
       </c>
       <c r="L7">
-        <v>2324.253849</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>2324.2538490000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>913.5798739000001</v>
+        <v>913.57987390000005</v>
       </c>
       <c r="C8">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D8">
-        <v>305.7473362</v>
+        <v>305.74733620000001</v>
       </c>
       <c r="E8">
-        <v>94.42961198</v>
+        <v>94.429611980000004</v>
       </c>
       <c r="F8">
-        <v>180.5162137</v>
+        <v>180.51621370000001</v>
       </c>
       <c r="G8">
-        <v>110.5865442</v>
+        <v>110.58654420000001</v>
       </c>
       <c r="H8">
-        <v>105.6040798</v>
+        <v>105.60407979999999</v>
       </c>
       <c r="I8">
         <v>5443.407612</v>
       </c>
       <c r="J8">
-        <v>5738.738399</v>
+        <v>5738.7383989999998</v>
       </c>
       <c r="K8">
         <v>6420.318064</v>
       </c>
       <c r="L8">
-        <v>7375.70317</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>7375.7031699999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>913.5797064</v>
+        <v>913.57970639999996</v>
       </c>
       <c r="C9">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D9">
-        <v>305.7768786</v>
+        <v>305.77687859999997</v>
       </c>
       <c r="E9">
-        <v>460.345401</v>
+        <v>460.34540099999998</v>
       </c>
       <c r="F9">
-        <v>614.6694877</v>
+        <v>614.66948769999999</v>
       </c>
       <c r="G9">
-        <v>524.5467748</v>
+        <v>524.54677479999998</v>
       </c>
       <c r="H9">
-        <v>530.1942424</v>
+        <v>530.19424240000001</v>
       </c>
       <c r="I9">
-        <v>7340.287958</v>
+        <v>7340.2879579999999</v>
       </c>
       <c r="J9">
-        <v>7544.256545</v>
+        <v>7544.2565450000002</v>
       </c>
       <c r="K9">
-        <v>8326.419330999999</v>
+        <v>8326.4193309999991</v>
       </c>
       <c r="L9">
         <v>9572.160468</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>911.5653354</v>
+        <v>911.56533539999998</v>
       </c>
       <c r="C10">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D10">
-        <v>304.3786593</v>
+        <v>304.37865929999998</v>
       </c>
       <c r="E10">
-        <v>2474.892731</v>
+        <v>2474.8927309999999</v>
       </c>
       <c r="F10">
-        <v>3182.755843</v>
+        <v>3182.7558429999999</v>
       </c>
       <c r="G10">
-        <v>2840.325766</v>
+        <v>2840.3257659999999</v>
       </c>
       <c r="H10">
-        <v>2696.99429</v>
+        <v>2696.9942900000001</v>
       </c>
       <c r="I10">
-        <v>5086.555269</v>
+        <v>5086.5552690000004</v>
       </c>
       <c r="J10">
         <v>4749.953888</v>
       </c>
       <c r="K10">
-        <v>5284.703183</v>
+        <v>5284.7031829999996</v>
       </c>
       <c r="L10">
-        <v>5863.927579</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>5863.9275790000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>911.5638353000001</v>
+        <v>911.56383530000005</v>
       </c>
       <c r="C11">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D11">
-        <v>302.9379678</v>
+        <v>302.93796780000002</v>
       </c>
       <c r="E11">
-        <v>75.83609752</v>
+        <v>75.836097519999996</v>
       </c>
       <c r="F11">
         <v>123.8849189</v>
       </c>
       <c r="G11">
-        <v>103.4854226</v>
+        <v>103.48542260000001</v>
       </c>
       <c r="H11">
-        <v>96.73323829</v>
+        <v>96.733238290000003</v>
       </c>
       <c r="I11">
         <v>4010.510781</v>
       </c>
       <c r="J11">
-        <v>3999.992496</v>
+        <v>3999.9924959999998</v>
       </c>
       <c r="K11">
-        <v>4469.111015</v>
+        <v>4469.1110150000004</v>
       </c>
       <c r="L11">
-        <v>4945.177076</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>4945.1770759999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>894.621042</v>
+        <v>894.62104199999999</v>
       </c>
       <c r="C12">
-        <v>6.361766667</v>
+        <v>6.3617666670000004</v>
       </c>
       <c r="D12">
-        <v>303.0519465</v>
+        <v>303.05194649999999</v>
       </c>
       <c r="E12">
-        <v>209.2735033</v>
+        <v>209.27350329999999</v>
       </c>
       <c r="F12">
-        <v>270.1383357</v>
+        <v>270.13833570000003</v>
       </c>
       <c r="G12">
-        <v>286.4112355</v>
+        <v>286.41123549999998</v>
       </c>
       <c r="H12">
-        <v>257.4433427</v>
+        <v>257.44334270000002</v>
       </c>
       <c r="I12">
-        <v>1917.498808</v>
+        <v>1917.4988080000001</v>
       </c>
       <c r="J12">
         <v>2040.660149</v>
       </c>
       <c r="K12">
-        <v>2123.216832</v>
+        <v>2123.2168320000001</v>
       </c>
       <c r="L12">
-        <v>2163.935976</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>2163.9359760000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>894.6202514</v>
+        <v>894.62025140000003</v>
       </c>
       <c r="C13">
-        <v>6.361766667</v>
+        <v>6.3617666670000004</v>
       </c>
       <c r="D13">
-        <v>304.4330024</v>
+        <v>304.43300240000002</v>
       </c>
       <c r="E13">
-        <v>60.35712732</v>
+        <v>60.357127319999996</v>
       </c>
       <c r="F13">
-        <v>99.34594561</v>
+        <v>99.345945610000001</v>
       </c>
       <c r="G13">
-        <v>95.32658948</v>
+        <v>95.326589479999996</v>
       </c>
       <c r="H13">
-        <v>89.24295100000001</v>
+        <v>89.242951000000005</v>
       </c>
       <c r="I13">
         <v>1665.9319</v>
@@ -1091,141 +1074,141 @@
         <v>1922.345863</v>
       </c>
       <c r="L13">
-        <v>1958.565238</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>1958.5652379999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>885.690128</v>
+        <v>885.69012799999996</v>
       </c>
       <c r="C14">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D14">
-        <v>295.9597281</v>
+        <v>295.95972810000001</v>
       </c>
       <c r="E14">
         <v>0.123379615</v>
       </c>
       <c r="F14">
-        <v>1.305029485</v>
+        <v>1.3050294849999999</v>
       </c>
       <c r="G14">
-        <v>0.94931276</v>
+        <v>0.94931275999999998</v>
       </c>
       <c r="H14">
         <v>1.058009022</v>
       </c>
       <c r="I14">
-        <v>3812.526833</v>
+        <v>3812.5268329999999</v>
       </c>
       <c r="J14">
         <v>3883.229871</v>
       </c>
       <c r="K14">
-        <v>3988.09554</v>
+        <v>3988.0955399999998</v>
       </c>
       <c r="L14">
-        <v>4685.870496</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>4685.8704959999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>885.6894797</v>
+        <v>885.68947969999999</v>
       </c>
       <c r="C15">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D15">
-        <v>295.990112</v>
+        <v>295.99011200000001</v>
       </c>
       <c r="E15">
-        <v>297.4561264</v>
+        <v>297.45612640000002</v>
       </c>
       <c r="F15">
-        <v>356.3740878</v>
+        <v>356.37408779999998</v>
       </c>
       <c r="G15">
-        <v>286.4841871</v>
+        <v>286.48418709999999</v>
       </c>
       <c r="H15">
-        <v>268.7736358</v>
+        <v>268.77363580000002</v>
       </c>
       <c r="I15">
-        <v>4130.06045</v>
+        <v>4130.0604499999999</v>
       </c>
       <c r="J15">
-        <v>4662.229254</v>
+        <v>4662.2292539999999</v>
       </c>
       <c r="K15">
-        <v>4532.709064</v>
+        <v>4532.7090639999997</v>
       </c>
       <c r="L15">
-        <v>5603.726472</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>5603.7264720000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>885.5490362</v>
+        <v>885.54903620000005</v>
       </c>
       <c r="C16">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D16">
         <v>295.9604334</v>
       </c>
       <c r="E16">
-        <v>807.5244887</v>
+        <v>807.52448870000001</v>
       </c>
       <c r="F16">
-        <v>814.4737917</v>
+        <v>814.47379169999999</v>
       </c>
       <c r="G16">
-        <v>758.517169</v>
+        <v>758.51716899999997</v>
       </c>
       <c r="H16">
-        <v>789.9448698</v>
+        <v>789.94486979999999</v>
       </c>
       <c r="I16">
-        <v>70081.60765000001</v>
+        <v>70081.607650000005</v>
       </c>
       <c r="J16">
-        <v>71066.41671</v>
+        <v>71066.416710000005</v>
       </c>
       <c r="K16">
-        <v>75297.14617000001</v>
+        <v>75297.146170000007</v>
       </c>
       <c r="L16">
-        <v>82850.34758</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>82850.347580000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>883.5352271</v>
+        <v>883.53522710000004</v>
       </c>
       <c r="C17">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D17">
-        <v>294.5696129</v>
+        <v>294.56961289999998</v>
       </c>
       <c r="E17">
         <v>24933.07288</v>
       </c>
       <c r="F17">
-        <v>28630.14259</v>
+        <v>28630.142589999999</v>
       </c>
       <c r="G17">
         <v>26721.37427</v>
@@ -1234,33 +1217,33 @@
         <v>25261.35759</v>
       </c>
       <c r="I17">
-        <v>35853.51811</v>
+        <v>35853.518109999997</v>
       </c>
       <c r="J17">
-        <v>34602.09316</v>
+        <v>34602.093159999997</v>
       </c>
       <c r="K17">
-        <v>36199.82513</v>
+        <v>36199.825129999997</v>
       </c>
       <c r="L17">
-        <v>39525.54815</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>39525.548150000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>883.5336557000001</v>
+        <v>883.53365570000005</v>
       </c>
       <c r="C18">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D18">
-        <v>291.6665676</v>
+        <v>291.66656760000001</v>
       </c>
       <c r="E18">
-        <v>395.6988722</v>
+        <v>395.69887219999998</v>
       </c>
       <c r="F18">
         <v>455.0363084</v>
@@ -1269,343 +1252,343 @@
         <v>425.3166296</v>
       </c>
       <c r="H18">
-        <v>364.3335305</v>
+        <v>364.33353049999999</v>
       </c>
       <c r="I18">
-        <v>26922.11674</v>
+        <v>26922.116740000001</v>
       </c>
       <c r="J18">
         <v>27365.74468</v>
       </c>
       <c r="K18">
-        <v>29171.58619</v>
+        <v>29171.586190000002</v>
       </c>
       <c r="L18">
         <v>31106.70046</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>883.5334743</v>
+        <v>883.53347429999997</v>
       </c>
       <c r="C19">
         <v>1.052566667</v>
       </c>
       <c r="D19">
-        <v>291.6665685</v>
+        <v>291.66656849999998</v>
       </c>
       <c r="E19">
-        <v>503.678298</v>
+        <v>503.67829799999998</v>
       </c>
       <c r="F19">
-        <v>588.600522</v>
+        <v>588.60052199999996</v>
       </c>
       <c r="G19">
-        <v>540.1770797</v>
+        <v>540.17707970000004</v>
       </c>
       <c r="H19">
         <v>511.6458207</v>
       </c>
       <c r="I19">
-        <v>28758.23354</v>
+        <v>28758.233540000001</v>
       </c>
       <c r="J19">
-        <v>28312.63188</v>
+        <v>28312.631880000001</v>
       </c>
       <c r="K19">
-        <v>28761.96782</v>
+        <v>28761.967820000002</v>
       </c>
       <c r="L19">
-        <v>36728.28442</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>36728.284420000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>883.5331863</v>
+        <v>883.53318630000001</v>
       </c>
       <c r="C20">
         <v>1.052566667</v>
       </c>
       <c r="D20">
-        <v>290.255055</v>
+        <v>290.25505500000003</v>
       </c>
       <c r="E20">
         <v>3702.925107</v>
       </c>
       <c r="F20">
-        <v>4618.742969</v>
+        <v>4618.7429689999999</v>
       </c>
       <c r="G20">
-        <v>3987.209674</v>
+        <v>3987.2096740000002</v>
       </c>
       <c r="H20">
-        <v>3481.19456</v>
+        <v>3481.1945599999999</v>
       </c>
       <c r="I20">
-        <v>31359.26876</v>
+        <v>31359.268759999999</v>
       </c>
       <c r="J20">
         <v>30806.87386</v>
       </c>
       <c r="K20">
-        <v>31197.29499</v>
+        <v>31197.294989999999</v>
       </c>
       <c r="L20">
-        <v>39952.23091</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>39952.230909999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>879.5121109</v>
+        <v>879.51211090000004</v>
       </c>
       <c r="C21">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D21">
-        <v>294.5594307</v>
+        <v>294.55943070000001</v>
       </c>
       <c r="E21">
-        <v>6230.947853</v>
+        <v>6230.9478529999997</v>
       </c>
       <c r="F21">
         <v>7050.93815</v>
       </c>
       <c r="G21">
-        <v>6336.573548</v>
+        <v>6336.5735480000003</v>
       </c>
       <c r="H21">
-        <v>6066.191524</v>
+        <v>6066.1915239999998</v>
       </c>
       <c r="I21">
-        <v>78624.15661999999</v>
+        <v>78624.156619999994</v>
       </c>
       <c r="J21">
         <v>79707.71686</v>
       </c>
       <c r="K21">
-        <v>84702.07283999999</v>
+        <v>84702.072839999993</v>
       </c>
       <c r="L21">
-        <v>92767.02963999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>92767.029639999993</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>871.5357706</v>
+        <v>871.53577059999998</v>
       </c>
       <c r="C22">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D22">
-        <v>288.8703973</v>
+        <v>288.87039729999998</v>
       </c>
       <c r="E22">
-        <v>1960.647779</v>
+        <v>1960.6477789999999</v>
       </c>
       <c r="F22">
         <v>2280.123423</v>
       </c>
       <c r="G22">
-        <v>2038.803309</v>
+        <v>2038.8033089999999</v>
       </c>
       <c r="H22">
-        <v>1924.73093</v>
+        <v>1924.7309299999999</v>
       </c>
       <c r="I22">
-        <v>4902.913953</v>
+        <v>4902.9139530000002</v>
       </c>
       <c r="J22">
-        <v>5082.679102</v>
+        <v>5082.6791020000001</v>
       </c>
       <c r="K22">
-        <v>5246.917479</v>
+        <v>5246.9174789999997</v>
       </c>
       <c r="L22">
-        <v>5641.950587</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>5641.9505870000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>871.5336416</v>
+        <v>871.53364160000001</v>
       </c>
       <c r="C23">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D23">
-        <v>290.2850108</v>
+        <v>290.28501080000001</v>
       </c>
       <c r="E23">
-        <v>400.9811296</v>
+        <v>400.98112959999997</v>
       </c>
       <c r="F23">
-        <v>439.3041554</v>
+        <v>439.30415540000001</v>
       </c>
       <c r="G23">
         <v>417.7473736</v>
       </c>
       <c r="H23">
-        <v>409.3625309</v>
+        <v>409.36253090000002</v>
       </c>
       <c r="I23">
-        <v>3213.220696</v>
+        <v>3213.2206959999999</v>
       </c>
       <c r="J23">
-        <v>3309.605879</v>
+        <v>3309.6058790000002</v>
       </c>
       <c r="K23">
-        <v>3480.900342</v>
+        <v>3480.9003419999999</v>
       </c>
       <c r="L23">
-        <v>3751.859486</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>3751.8594859999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>871.4562521</v>
+        <v>871.45625210000003</v>
       </c>
       <c r="C24">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D24">
-        <v>293.170627</v>
+        <v>293.17062700000002</v>
       </c>
       <c r="E24">
-        <v>4294.564286</v>
+        <v>4294.5642859999998</v>
       </c>
       <c r="F24">
         <v>4707.157843</v>
       </c>
       <c r="G24">
-        <v>4352.886747</v>
+        <v>4352.8867469999996</v>
       </c>
       <c r="H24">
-        <v>4053.68315</v>
+        <v>4053.6831499999998</v>
       </c>
       <c r="I24">
-        <v>1354.953279</v>
+        <v>1354.9532790000001</v>
       </c>
       <c r="J24">
-        <v>1374.970146</v>
+        <v>1374.9701460000001</v>
       </c>
       <c r="K24">
-        <v>1423.074049</v>
+        <v>1423.0740490000001</v>
       </c>
       <c r="L24">
         <v>1410.388588</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>871.4088508</v>
+        <v>871.40885079999998</v>
       </c>
       <c r="C25">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D25">
-        <v>298.8285361</v>
+        <v>298.82853610000001</v>
       </c>
       <c r="E25">
-        <v>465.5193412</v>
+        <v>465.51934119999999</v>
       </c>
       <c r="F25">
-        <v>514.1657405</v>
+        <v>514.16574049999997</v>
       </c>
       <c r="G25">
-        <v>489.1704664</v>
+        <v>489.17046640000001</v>
       </c>
       <c r="H25">
-        <v>422.372631</v>
+        <v>422.37263100000001</v>
       </c>
       <c r="I25">
         <v>2821.137213</v>
       </c>
       <c r="J25">
-        <v>2829.177855</v>
+        <v>2829.1778549999999</v>
       </c>
       <c r="K25">
-        <v>2784.113306</v>
+        <v>2784.1133060000002</v>
       </c>
       <c r="L25">
-        <v>3422.533051</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>3422.5330509999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>871.1278417</v>
+        <v>871.12784169999998</v>
       </c>
       <c r="C26">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D26">
         <v>297.4360203</v>
       </c>
       <c r="E26">
-        <v>2040.106339</v>
+        <v>2040.1063389999999</v>
       </c>
       <c r="F26">
-        <v>2515.234803</v>
+        <v>2515.2348029999998</v>
       </c>
       <c r="G26">
         <v>2386.028323</v>
       </c>
       <c r="H26">
-        <v>2045.142868</v>
+        <v>2045.1428679999999</v>
       </c>
       <c r="I26">
-        <v>439.0806795</v>
+        <v>439.08067949999997</v>
       </c>
       <c r="J26">
         <v>367.9869885</v>
       </c>
       <c r="K26">
-        <v>313.9463776</v>
+        <v>313.94637760000001</v>
       </c>
       <c r="L26">
         <v>378.5207724</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>866.5924716</v>
+        <v>866.59247159999995</v>
       </c>
       <c r="C27">
-        <v>6.361766667</v>
+        <v>6.3617666670000004</v>
       </c>
       <c r="D27">
-        <v>296.0889527</v>
+        <v>296.08895269999999</v>
       </c>
       <c r="E27">
-        <v>1188.651581</v>
+        <v>1188.6515810000001</v>
       </c>
       <c r="F27">
-        <v>1309.529967</v>
+        <v>1309.5299669999999</v>
       </c>
       <c r="G27">
         <v>1423.597303</v>
@@ -1614,42 +1597,42 @@
         <v>1374.711892</v>
       </c>
       <c r="I27">
-        <v>4122.770095</v>
+        <v>4122.7700949999999</v>
       </c>
       <c r="J27">
-        <v>4426.576576</v>
+        <v>4426.5765760000004</v>
       </c>
       <c r="K27">
-        <v>4661.35487</v>
+        <v>4661.3548700000001</v>
       </c>
       <c r="L27">
-        <v>4598.345368</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>4598.3453680000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>866.5918081</v>
+        <v>866.59180809999998</v>
       </c>
       <c r="C28">
-        <v>6.361766667</v>
+        <v>6.3617666670000004</v>
       </c>
       <c r="D28">
-        <v>296.0572448</v>
+        <v>296.05724479999998</v>
       </c>
       <c r="E28">
-        <v>66.96754531000001</v>
+        <v>66.967545310000006</v>
       </c>
       <c r="F28">
-        <v>75.64200267</v>
+        <v>75.642002669999997</v>
       </c>
       <c r="G28">
-        <v>57.80298697</v>
+        <v>57.802986969999999</v>
       </c>
       <c r="H28">
-        <v>63.05648001</v>
+        <v>63.056480010000001</v>
       </c>
       <c r="I28">
         <v>3347.700848</v>
@@ -1658,51 +1641,51 @@
         <v>3608.845722</v>
       </c>
       <c r="K28">
-        <v>3897.165149</v>
+        <v>3897.1651489999999</v>
       </c>
       <c r="L28">
-        <v>3857.633179</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>3857.6331789999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>863.5746885999999</v>
+        <v>863.57468859999994</v>
       </c>
       <c r="C29">
-        <v>6.415366667</v>
+        <v>6.4153666669999998</v>
       </c>
       <c r="D29">
-        <v>297.5335833</v>
+        <v>297.53358329999998</v>
       </c>
       <c r="E29">
-        <v>3317.177691</v>
+        <v>3317.1776909999999</v>
       </c>
       <c r="F29">
-        <v>3397.710084</v>
+        <v>3397.7100839999998</v>
       </c>
       <c r="G29">
         <v>3773.062375</v>
       </c>
       <c r="H29">
-        <v>3592.995155</v>
+        <v>3592.9951550000001</v>
       </c>
       <c r="I29">
-        <v>1770.177059</v>
+        <v>1770.1770590000001</v>
       </c>
       <c r="J29">
         <v>1737.749249</v>
       </c>
       <c r="K29">
-        <v>1679.404649</v>
+        <v>1679.4046490000001</v>
       </c>
       <c r="L29">
         <v>1711.646536</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1710,22 +1693,22 @@
         <v>863.5729771</v>
       </c>
       <c r="C30">
-        <v>6.415366667</v>
+        <v>6.4153666669999998</v>
       </c>
       <c r="D30">
-        <v>300.3485893</v>
+        <v>300.34858930000001</v>
       </c>
       <c r="E30">
-        <v>442.3136966</v>
+        <v>442.31369660000001</v>
       </c>
       <c r="F30">
-        <v>554.6837957</v>
+        <v>554.68379570000002</v>
       </c>
       <c r="G30">
-        <v>537.2650538</v>
+        <v>537.26505380000003</v>
       </c>
       <c r="H30">
-        <v>506.0809935</v>
+        <v>506.08099349999998</v>
       </c>
       <c r="I30">
         <v>1815.630136</v>
@@ -1734,62 +1717,62 @@
         <v>1932.093286</v>
       </c>
       <c r="K30">
-        <v>2018.909511</v>
+        <v>2018.9095110000001</v>
       </c>
       <c r="L30">
         <v>2029.645906</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>852.5517245</v>
+        <v>852.55172449999998</v>
       </c>
       <c r="C31">
-        <v>3.467233333</v>
+        <v>3.4672333329999998</v>
       </c>
       <c r="D31">
         <v>290.3831217</v>
       </c>
       <c r="E31">
-        <v>15284.0277</v>
+        <v>15284.027700000001</v>
       </c>
       <c r="F31">
         <v>17617.30341</v>
       </c>
       <c r="G31">
-        <v>15583.65807</v>
+        <v>15583.658069999999</v>
       </c>
       <c r="H31">
-        <v>14456.82405</v>
+        <v>14456.824049999999</v>
       </c>
       <c r="I31">
         <v>10177.84189</v>
       </c>
       <c r="J31">
-        <v>9835.327101000001</v>
+        <v>9835.3271010000008</v>
       </c>
       <c r="K31">
         <v>10585.21012</v>
       </c>
       <c r="L31">
-        <v>10676.54791</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+        <v>10676.547909999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32">
-        <v>852.4876705</v>
+        <v>852.48767050000004</v>
       </c>
       <c r="C32">
-        <v>3.467233333</v>
+        <v>3.4672333329999998</v>
       </c>
       <c r="D32">
-        <v>284.6111068</v>
+        <v>284.61110680000002</v>
       </c>
       <c r="E32">
         <v>14598.42935</v>
@@ -1804,36 +1787,36 @@
         <v>13289.84489</v>
       </c>
       <c r="I32">
-        <v>5823.327791</v>
+        <v>5823.3277909999997</v>
       </c>
       <c r="J32">
-        <v>5604.678192</v>
+        <v>5604.6781920000003</v>
       </c>
       <c r="K32">
-        <v>5522.580398</v>
+        <v>5522.5803980000001</v>
       </c>
       <c r="L32">
-        <v>5709.83144</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
+        <v>5709.8314399999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>850.561693</v>
+        <v>850.56169299999999</v>
       </c>
       <c r="C33">
         <v>0.897416667</v>
       </c>
       <c r="D33">
-        <v>291.8683606</v>
+        <v>291.86836060000002</v>
       </c>
       <c r="E33">
         <v>1065.395043</v>
       </c>
       <c r="F33">
-        <v>1193.014346</v>
+        <v>1193.0143459999999</v>
       </c>
       <c r="G33">
         <v>1095.722088</v>
@@ -1848,74 +1831,74 @@
         <v>2876.028151</v>
       </c>
       <c r="K33">
-        <v>3036.341311</v>
+        <v>3036.3413110000001</v>
       </c>
       <c r="L33">
         <v>3297.697842</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>850.5612583</v>
+        <v>850.56125829999996</v>
       </c>
       <c r="C34">
         <v>0.897416667</v>
       </c>
       <c r="D34">
-        <v>291.8359443</v>
+        <v>291.83594429999999</v>
       </c>
       <c r="E34">
-        <v>376.3391602</v>
+        <v>376.33916019999998</v>
       </c>
       <c r="F34">
-        <v>414.3230937</v>
+        <v>414.32309370000002</v>
       </c>
       <c r="G34">
-        <v>397.1499246</v>
+        <v>397.14992460000002</v>
       </c>
       <c r="H34">
-        <v>383.1275732</v>
+        <v>383.12757319999997</v>
       </c>
       <c r="I34">
-        <v>1562.460021</v>
+        <v>1562.4600210000001</v>
       </c>
       <c r="J34">
-        <v>1780.212602</v>
+        <v>1780.2126020000001</v>
       </c>
       <c r="K34">
-        <v>2093.119697</v>
+        <v>2093.1196970000001</v>
       </c>
       <c r="L34">
-        <v>2295.545299</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
+        <v>2295.5452989999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35">
-        <v>828.570821</v>
+        <v>828.57082100000002</v>
       </c>
       <c r="C35">
         <v>0.897416667</v>
       </c>
       <c r="D35">
-        <v>283.2464333</v>
+        <v>283.24643329999998</v>
       </c>
       <c r="E35">
-        <v>350.6093824</v>
+        <v>350.60938240000002</v>
       </c>
       <c r="F35">
-        <v>384.5149429</v>
+        <v>384.51494289999999</v>
       </c>
       <c r="G35">
-        <v>369.8230572</v>
+        <v>369.82305719999999</v>
       </c>
       <c r="H35">
-        <v>354.0175457</v>
+        <v>354.01754570000003</v>
       </c>
       <c r="I35">
         <v>1960.768401</v>
@@ -1924,144 +1907,144 @@
         <v>2383.324603</v>
       </c>
       <c r="K35">
-        <v>2583.612949</v>
+        <v>2583.6129489999998</v>
       </c>
       <c r="L35">
-        <v>2891.339424</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
+        <v>2891.3394239999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>828.5707407</v>
+        <v>828.57074069999999</v>
       </c>
       <c r="C36">
         <v>0.897416667</v>
       </c>
       <c r="D36">
-        <v>283.2795467</v>
+        <v>283.27954670000003</v>
       </c>
       <c r="E36">
-        <v>822.8943736</v>
+        <v>822.89437359999999</v>
       </c>
       <c r="F36">
-        <v>856.6218165</v>
+        <v>856.62181650000002</v>
       </c>
       <c r="G36">
-        <v>777.6360213</v>
+        <v>777.63602130000004</v>
       </c>
       <c r="H36">
-        <v>752.0087366</v>
+        <v>752.00873660000002</v>
       </c>
       <c r="I36">
-        <v>5159.597511</v>
+        <v>5159.5975109999999</v>
       </c>
       <c r="J36">
-        <v>6053.055109</v>
+        <v>6053.0551089999999</v>
       </c>
       <c r="K36">
-        <v>6525.261936</v>
+        <v>6525.2619359999999</v>
       </c>
       <c r="L36">
-        <v>7298.381189</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
+        <v>7298.3811889999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37">
-        <v>797.5450976</v>
+        <v>797.54509759999996</v>
       </c>
       <c r="C37">
-        <v>1.707</v>
+        <v>1.7070000000000001</v>
       </c>
       <c r="D37">
-        <v>279.0507536</v>
+        <v>279.05075360000001</v>
       </c>
       <c r="E37">
-        <v>2185.274515</v>
+        <v>2185.2745150000001</v>
       </c>
       <c r="F37">
         <v>2564.926062</v>
       </c>
       <c r="G37">
-        <v>2446.582728</v>
+        <v>2446.5827279999999</v>
       </c>
       <c r="H37">
-        <v>2351.577438</v>
+        <v>2351.5774379999998</v>
       </c>
       <c r="I37">
         <v>12063.56849</v>
       </c>
       <c r="J37">
-        <v>10943.58254</v>
+        <v>10943.582539999999</v>
       </c>
       <c r="K37">
-        <v>8445.257814000001</v>
+        <v>8445.2578140000005</v>
       </c>
       <c r="L37">
-        <v>8578.82099</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
+        <v>8578.8209900000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38">
-        <v>797.529183</v>
+        <v>797.52918299999999</v>
       </c>
       <c r="C38">
-        <v>1.707</v>
+        <v>1.7070000000000001</v>
       </c>
       <c r="D38">
-        <v>279.01571</v>
+        <v>279.01571000000001</v>
       </c>
       <c r="E38">
-        <v>573.1981833</v>
+        <v>573.19818329999998</v>
       </c>
       <c r="F38">
-        <v>567.0383143</v>
+        <v>567.03831430000002</v>
       </c>
       <c r="G38">
-        <v>501.8263299</v>
+        <v>501.82632990000002</v>
       </c>
       <c r="H38">
-        <v>539.2860728000001</v>
+        <v>539.28607280000006</v>
       </c>
       <c r="I38">
-        <v>6140.136248</v>
+        <v>6140.1362479999998</v>
       </c>
       <c r="J38">
-        <v>5492.064663</v>
+        <v>5492.0646630000001</v>
       </c>
       <c r="K38">
-        <v>4154.648771</v>
+        <v>4154.6487710000001</v>
       </c>
       <c r="L38">
-        <v>4120.445296</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
+        <v>4120.4452959999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39">
-        <v>794.570152</v>
+        <v>794.57015200000001</v>
       </c>
       <c r="C39">
-        <v>5.174133333</v>
+        <v>5.1741333330000003</v>
       </c>
       <c r="D39">
-        <v>280.5053798</v>
+        <v>280.50537980000001</v>
       </c>
       <c r="E39">
-        <v>87.94496404</v>
+        <v>87.944964040000002</v>
       </c>
       <c r="F39">
-        <v>93.20704048</v>
+        <v>93.207040480000003</v>
       </c>
       <c r="G39">
         <v>115.3118511</v>
@@ -2070,71 +2053,71 @@
         <v>101.3000656</v>
       </c>
       <c r="I39">
-        <v>2751.797232</v>
+        <v>2751.7972319999999</v>
       </c>
       <c r="J39">
         <v>3675.159858</v>
       </c>
       <c r="K39">
-        <v>4230.056145</v>
+        <v>4230.0561449999996</v>
       </c>
       <c r="L39">
         <v>4806.458455</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40">
-        <v>794.5697036</v>
+        <v>794.56970360000003</v>
       </c>
       <c r="C40">
-        <v>5.174133333</v>
+        <v>5.1741333330000003</v>
       </c>
       <c r="D40">
-        <v>279.0682617</v>
+        <v>279.06826169999999</v>
       </c>
       <c r="E40">
-        <v>884.99465</v>
+        <v>884.99464999999998</v>
       </c>
       <c r="F40">
-        <v>951.8497252</v>
+        <v>951.84972519999997</v>
       </c>
       <c r="G40">
-        <v>953.5571483</v>
+        <v>953.55714829999999</v>
       </c>
       <c r="H40">
-        <v>916.5285077</v>
+        <v>916.52850769999998</v>
       </c>
       <c r="I40">
-        <v>3570.14573</v>
+        <v>3570.1457300000002</v>
       </c>
       <c r="J40">
         <v>4605.285766</v>
       </c>
       <c r="K40">
-        <v>5309.268135</v>
+        <v>5309.2681350000003</v>
       </c>
       <c r="L40">
-        <v>6079.926061</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12">
+        <v>6079.9260610000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41">
-        <v>792.5553609999999</v>
+        <v>792.55536099999995</v>
       </c>
       <c r="C41">
-        <v>5.174133333</v>
+        <v>5.1741333330000003</v>
       </c>
       <c r="D41">
-        <v>277.603675</v>
+        <v>277.60367500000001</v>
       </c>
       <c r="E41">
-        <v>1363.284068</v>
+        <v>1363.2840679999999</v>
       </c>
       <c r="F41">
         <v>1446.836335</v>
@@ -2146,7 +2129,7 @@
         <v>1370.151429</v>
       </c>
       <c r="I41">
-        <v>2345.175272</v>
+        <v>2345.1752719999999</v>
       </c>
       <c r="J41">
         <v>2911.441065</v>
@@ -2155,194 +2138,194 @@
         <v>3487.791256</v>
       </c>
       <c r="L41">
-        <v>4002.39985</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
+        <v>4002.3998499999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42">
-        <v>792.5547683999999</v>
+        <v>792.55476839999994</v>
       </c>
       <c r="C42">
-        <v>5.174133333</v>
+        <v>5.1741333330000003</v>
       </c>
       <c r="D42">
-        <v>277.5682955</v>
+        <v>277.56829549999998</v>
       </c>
       <c r="E42">
-        <v>196.2849335</v>
+        <v>196.28493349999999</v>
       </c>
       <c r="F42">
-        <v>211.5919119</v>
+        <v>211.59191190000001</v>
       </c>
       <c r="G42">
-        <v>258.2846484</v>
+        <v>258.28464839999998</v>
       </c>
       <c r="H42">
-        <v>229.4186629</v>
+        <v>229.41866289999999</v>
       </c>
       <c r="I42">
-        <v>1954.563385</v>
+        <v>1954.5633849999999</v>
       </c>
       <c r="J42">
-        <v>2574.829285</v>
+        <v>2574.8292849999998</v>
       </c>
       <c r="K42">
-        <v>3138.934488</v>
+        <v>3138.9344879999999</v>
       </c>
       <c r="L42">
         <v>3615.636884</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43">
-        <v>766.5396204</v>
+        <v>766.53962039999999</v>
       </c>
       <c r="C43">
-        <v>5.174133333</v>
+        <v>5.1741333330000003</v>
       </c>
       <c r="D43">
-        <v>271.8146801</v>
+        <v>271.81468009999998</v>
       </c>
       <c r="E43">
-        <v>4104.214386</v>
+        <v>4104.2143859999996</v>
       </c>
       <c r="F43">
-        <v>5297.566865</v>
+        <v>5297.5668649999998</v>
       </c>
       <c r="G43">
-        <v>4641.612403</v>
+        <v>4641.6124030000001</v>
       </c>
       <c r="H43">
-        <v>4973.75238</v>
+        <v>4973.7523799999999</v>
       </c>
       <c r="I43">
-        <v>5940.627557</v>
+        <v>5940.6275569999998</v>
       </c>
       <c r="J43">
-        <v>7169.464484</v>
+        <v>7169.4644840000001</v>
       </c>
       <c r="K43">
-        <v>8052.187963</v>
+        <v>8052.1879630000003</v>
       </c>
       <c r="L43">
-        <v>8860.849448000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12">
+        <v>8860.8494480000008</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44">
-        <v>766.5392929</v>
+        <v>766.53929289999996</v>
       </c>
       <c r="C44">
-        <v>5.174133333</v>
+        <v>5.1741333330000003</v>
       </c>
       <c r="D44">
-        <v>271.7777128</v>
+        <v>271.77771280000002</v>
       </c>
       <c r="E44">
-        <v>368.5863285</v>
+        <v>368.58632849999998</v>
       </c>
       <c r="F44">
-        <v>411.3565981</v>
+        <v>411.35659809999999</v>
       </c>
       <c r="G44">
-        <v>423.448345</v>
+        <v>423.44834500000002</v>
       </c>
       <c r="H44">
-        <v>415.8182158</v>
+        <v>415.81821580000002</v>
       </c>
       <c r="I44">
-        <v>4653.351953</v>
+        <v>4653.3519530000003</v>
       </c>
       <c r="J44">
-        <v>5758.053828</v>
+        <v>5758.0538280000001</v>
       </c>
       <c r="K44">
-        <v>6231.472059</v>
+        <v>6231.4720589999997</v>
       </c>
       <c r="L44">
-        <v>7014.426233</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12">
+        <v>7014.4262330000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45">
-        <v>750.5435060999999</v>
+        <v>750.54350609999995</v>
       </c>
       <c r="C45">
-        <v>5.052833333</v>
+        <v>5.0528333329999997</v>
       </c>
       <c r="D45">
         <v>270.3798673</v>
       </c>
       <c r="E45">
-        <v>212.8541828</v>
+        <v>212.85418279999999</v>
       </c>
       <c r="F45">
-        <v>262.4123668</v>
+        <v>262.41236679999997</v>
       </c>
       <c r="G45">
-        <v>264.3691274</v>
+        <v>264.36912740000002</v>
       </c>
       <c r="H45">
-        <v>240.4887692</v>
+        <v>240.48876920000001</v>
       </c>
       <c r="I45">
-        <v>7032.271559</v>
+        <v>7032.2715589999998</v>
       </c>
       <c r="J45">
         <v>1996.913082</v>
       </c>
       <c r="K45">
-        <v>9849.981797</v>
+        <v>9849.9817970000004</v>
       </c>
       <c r="L45">
-        <v>10082.07513</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12">
+        <v>10082.075129999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46">
-        <v>750.5424202</v>
+        <v>750.54242020000004</v>
       </c>
       <c r="C46">
-        <v>5.052833333</v>
+        <v>5.0528333329999997</v>
       </c>
       <c r="D46">
-        <v>270.4181927</v>
+        <v>270.41819270000002</v>
       </c>
       <c r="E46">
-        <v>1393.209103</v>
+        <v>1393.2091029999999</v>
       </c>
       <c r="F46">
         <v>1580.141196</v>
       </c>
       <c r="G46">
-        <v>1534.513307</v>
+        <v>1534.5133069999999</v>
       </c>
       <c r="H46">
-        <v>1457.987416</v>
+        <v>1457.9874159999999</v>
       </c>
       <c r="I46">
-        <v>7927.794916</v>
+        <v>7927.7949159999998</v>
       </c>
       <c r="J46">
-        <v>2478.878079</v>
+        <v>2478.8780790000001</v>
       </c>
       <c r="K46">
-        <v>10840.86165</v>
+        <v>10840.861650000001</v>
       </c>
       <c r="L46">
         <v>11305.79098</v>
@@ -2354,14 +2337,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AH41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2462,53 +2447,53 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>967.5522655</v>
+        <v>967.55226549999998</v>
       </c>
       <c r="C2">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D2">
-        <v>312.5144217</v>
+        <v>312.51442170000001</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>967.5520752</v>
+        <v>967.55207519999999</v>
       </c>
       <c r="C3">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D3">
-        <v>312.4874341</v>
+        <v>312.48743409999997</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2516,70 +2501,70 @@
         <v>965.5342114</v>
       </c>
       <c r="C4">
-        <v>1.018716667</v>
+        <v>1.0187166670000001</v>
       </c>
       <c r="D4">
-        <v>308.3125788</v>
+        <v>308.31257879999998</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>965.5318508</v>
+        <v>965.53185080000003</v>
       </c>
       <c r="C5">
-        <v>1.018716667</v>
+        <v>1.0187166670000001</v>
       </c>
       <c r="D5">
-        <v>308.3393262</v>
+        <v>308.33932620000002</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>938.5822902</v>
+        <v>938.58229019999999</v>
       </c>
       <c r="C6">
-        <v>3.312083333</v>
+        <v>3.3120833329999999</v>
       </c>
       <c r="D6">
-        <v>301.4248499</v>
+        <v>301.42484990000003</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>938.5804534</v>
+        <v>938.58045340000001</v>
       </c>
       <c r="C7">
-        <v>3.312083333</v>
+        <v>3.3120833329999999</v>
       </c>
       <c r="D7">
         <v>302.8109753</v>
@@ -2588,211 +2573,211 @@
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>913.5798739000001</v>
+        <v>913.57987390000005</v>
       </c>
       <c r="C8">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D8">
-        <v>305.7473362</v>
+        <v>305.74733620000001</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>913.5797064</v>
+        <v>913.57970639999996</v>
       </c>
       <c r="C9">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D9">
-        <v>305.7768786</v>
+        <v>305.77687859999997</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>911.5653354</v>
+        <v>911.56533539999998</v>
       </c>
       <c r="C10">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D10">
-        <v>304.3786593</v>
+        <v>304.37865929999998</v>
       </c>
       <c r="E10" t="s">
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>911.5638353000001</v>
+        <v>911.56383530000005</v>
       </c>
       <c r="C11">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D11">
-        <v>302.9379678</v>
+        <v>302.93796780000002</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>894.621042</v>
+        <v>894.62104199999999</v>
       </c>
       <c r="C12">
-        <v>6.361766667</v>
+        <v>6.3617666670000004</v>
       </c>
       <c r="D12">
-        <v>303.0519465</v>
+        <v>303.05194649999999</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" t="s">
         <v>47</v>
       </c>
-      <c r="H12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34">
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>894.6202514</v>
+        <v>894.62025140000003</v>
       </c>
       <c r="C13">
-        <v>6.361766667</v>
+        <v>6.3617666670000004</v>
       </c>
       <c r="D13">
-        <v>304.4330024</v>
+        <v>304.43300240000002</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" t="s">
         <v>47</v>
       </c>
-      <c r="I13" t="s">
-        <v>61</v>
-      </c>
-      <c r="J13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34">
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>885.690128</v>
+        <v>885.69012799999996</v>
       </c>
       <c r="C14">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D14">
-        <v>295.9597281</v>
+        <v>295.95972810000001</v>
       </c>
       <c r="E14" t="s">
         <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>885.6894797</v>
+        <v>885.68947969999999</v>
       </c>
       <c r="C15">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D15">
-        <v>295.990112</v>
+        <v>295.99011200000001</v>
       </c>
       <c r="E15" t="s">
         <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>885.5490362</v>
+        <v>885.54903620000005</v>
       </c>
       <c r="C16">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D16">
         <v>295.9604334</v>
@@ -2801,892 +2786,747 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>883.5352271</v>
+        <v>883.53522710000004</v>
       </c>
       <c r="C17">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D17">
-        <v>294.5696129</v>
+        <v>294.56961289999998</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>883.5336557000001</v>
+        <v>883.53365570000005</v>
       </c>
       <c r="C18">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D18">
-        <v>291.6665676</v>
+        <v>291.66656760000001</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>883.5334743</v>
+        <v>883.53347429999997</v>
       </c>
       <c r="C19">
         <v>1.052566667</v>
       </c>
       <c r="D19">
-        <v>291.6665685</v>
+        <v>291.66656849999998</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
       </c>
       <c r="F19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>883.5331863</v>
+        <v>883.53318630000001</v>
       </c>
       <c r="C20">
         <v>1.052566667</v>
       </c>
       <c r="D20">
-        <v>290.255055</v>
+        <v>290.25505500000003</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>879.5121109</v>
+        <v>879.51211090000004</v>
       </c>
       <c r="C21">
-        <v>3.379783333</v>
+        <v>3.3797833329999998</v>
       </c>
       <c r="D21">
-        <v>294.5594307</v>
+        <v>294.55943070000001</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G21" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>871.5357706</v>
+        <v>871.53577059999998</v>
       </c>
       <c r="C22">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D22">
-        <v>288.8703973</v>
+        <v>288.87039729999998</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>871.5336416</v>
+        <v>871.53364160000001</v>
       </c>
       <c r="C23">
-        <v>3.413633333</v>
+        <v>3.4136333329999999</v>
       </c>
       <c r="D23">
-        <v>290.2850108</v>
+        <v>290.28501080000001</v>
       </c>
       <c r="E23" t="s">
         <v>13</v>
       </c>
       <c r="F23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B24">
-        <v>871.4562521</v>
+        <v>866.59247159999995</v>
       </c>
       <c r="C24">
-        <v>3.413633333</v>
+        <v>6.3617666670000004</v>
       </c>
       <c r="D24">
-        <v>293.170627</v>
+        <v>296.08895269999999</v>
       </c>
       <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A25" s="1">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>866.59180809999998</v>
+      </c>
+      <c r="C25">
+        <v>6.3617666670000004</v>
+      </c>
+      <c r="D25">
+        <v>296.05724479999998</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A26" s="1">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>863.57468859999994</v>
+      </c>
+      <c r="C26">
+        <v>6.4153666669999998</v>
+      </c>
+      <c r="D26">
+        <v>297.53358329999998</v>
+      </c>
+      <c r="E26" t="s">
         <v>13</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A27" s="1">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>863.5729771</v>
+      </c>
+      <c r="C27">
+        <v>6.4153666669999998</v>
+      </c>
+      <c r="D27">
+        <v>300.34858930000001</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A28" s="1">
         <v>31</v>
       </c>
-      <c r="G24" t="s">
+      <c r="B28">
+        <v>850.56169299999999</v>
+      </c>
+      <c r="C28">
+        <v>0.897416667</v>
+      </c>
+      <c r="D28">
+        <v>291.86836060000002</v>
+      </c>
+      <c r="E28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" t="s">
+        <v>30</v>
+      </c>
+      <c r="J28" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" t="s">
+        <v>30</v>
+      </c>
+      <c r="L28" t="s">
+        <v>30</v>
+      </c>
+      <c r="M28" t="s">
+        <v>30</v>
+      </c>
+      <c r="N28" t="s">
+        <v>49</v>
+      </c>
+      <c r="O28" t="s">
+        <v>30</v>
+      </c>
+      <c r="P28" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>30</v>
+      </c>
+      <c r="R28" t="s">
+        <v>30</v>
+      </c>
+      <c r="S28" t="s">
+        <v>30</v>
+      </c>
+      <c r="T28" t="s">
+        <v>30</v>
+      </c>
+      <c r="U28" t="s">
+        <v>30</v>
+      </c>
+      <c r="V28" t="s">
+        <v>30</v>
+      </c>
+      <c r="W28" t="s">
+        <v>30</v>
+      </c>
+      <c r="X28" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A29" s="1">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>850.56125829999996</v>
+      </c>
+      <c r="C29">
+        <v>0.897416667</v>
+      </c>
+      <c r="D29">
+        <v>291.83594429999999</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29" t="s">
+        <v>48</v>
+      </c>
+      <c r="K29" t="s">
+        <v>30</v>
+      </c>
+      <c r="L29" t="s">
+        <v>30</v>
+      </c>
+      <c r="M29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N29" t="s">
+        <v>49</v>
+      </c>
+      <c r="O29" t="s">
+        <v>30</v>
+      </c>
+      <c r="P29" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>30</v>
+      </c>
+      <c r="R29" t="s">
+        <v>30</v>
+      </c>
+      <c r="S29" t="s">
+        <v>30</v>
+      </c>
+      <c r="T29" t="s">
+        <v>30</v>
+      </c>
+      <c r="U29" t="s">
+        <v>30</v>
+      </c>
+      <c r="V29" t="s">
+        <v>30</v>
+      </c>
+      <c r="W29" t="s">
+        <v>30</v>
+      </c>
+      <c r="X29" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A30" s="1">
+        <v>33</v>
+      </c>
+      <c r="B30">
+        <v>828.57082100000002</v>
+      </c>
+      <c r="C30">
+        <v>0.897416667</v>
+      </c>
+      <c r="D30">
+        <v>283.24643329999998</v>
+      </c>
+      <c r="E30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J30" t="s">
+        <v>31</v>
+      </c>
+      <c r="K30" t="s">
+        <v>31</v>
+      </c>
+      <c r="L30" t="s">
+        <v>31</v>
+      </c>
+      <c r="M30" t="s">
+        <v>31</v>
+      </c>
+      <c r="N30" t="s">
         <v>50</v>
       </c>
-      <c r="H24" t="s">
-        <v>56</v>
-      </c>
-      <c r="I24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25">
-        <v>871.4088508</v>
-      </c>
-      <c r="C25">
-        <v>3.413633333</v>
-      </c>
-      <c r="D25">
-        <v>298.8285361</v>
-      </c>
-      <c r="E25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="O30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A31" s="1">
+        <v>34</v>
+      </c>
+      <c r="B31">
+        <v>828.57074069999999</v>
+      </c>
+      <c r="C31">
+        <v>0.897416667</v>
+      </c>
+      <c r="D31">
+        <v>283.27954670000003</v>
+      </c>
+      <c r="E31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K31" t="s">
+        <v>31</v>
+      </c>
+      <c r="L31" t="s">
+        <v>31</v>
+      </c>
+      <c r="M31" t="s">
+        <v>31</v>
+      </c>
+      <c r="N31" t="s">
+        <v>50</v>
+      </c>
+      <c r="O31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A32" s="1">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>797.54509759999996</v>
+      </c>
+      <c r="C32">
+        <v>1.7070000000000001</v>
+      </c>
+      <c r="D32">
+        <v>279.05075360000001</v>
+      </c>
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" t="s">
         <v>32</v>
       </c>
-      <c r="G25" t="s">
-        <v>51</v>
-      </c>
-      <c r="H25" t="s">
-        <v>57</v>
-      </c>
-      <c r="I25" t="s">
-        <v>63</v>
-      </c>
-      <c r="J25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>871.1278417</v>
-      </c>
-      <c r="C26">
-        <v>3.413633333</v>
-      </c>
-      <c r="D26">
-        <v>297.4360203</v>
-      </c>
-      <c r="E26" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" t="s">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="1">
+        <v>36</v>
+      </c>
+      <c r="B33">
+        <v>797.52918299999999</v>
+      </c>
+      <c r="C33">
+        <v>1.7070000000000001</v>
+      </c>
+      <c r="D33">
+        <v>279.01571000000001</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27">
-        <v>866.5924716</v>
-      </c>
-      <c r="C27">
-        <v>6.361766667</v>
-      </c>
-      <c r="D27">
-        <v>296.0889527</v>
-      </c>
-      <c r="E27" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="1">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>794.57015200000001</v>
+      </c>
+      <c r="C34">
+        <v>5.1741333330000003</v>
+      </c>
+      <c r="D34">
+        <v>280.50537980000001</v>
+      </c>
+      <c r="E34" t="s">
         <v>15</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28">
-        <v>866.5918081</v>
-      </c>
-      <c r="C28">
-        <v>6.361766667</v>
-      </c>
-      <c r="D28">
-        <v>296.0572448</v>
-      </c>
-      <c r="E28" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="1">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>794.56970360000003</v>
+      </c>
+      <c r="C35">
+        <v>5.1741333330000003</v>
+      </c>
+      <c r="D35">
+        <v>279.06826169999999</v>
+      </c>
+      <c r="E35" t="s">
         <v>15</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="B29">
-        <v>863.5746885999999</v>
-      </c>
-      <c r="C29">
-        <v>6.415366667</v>
-      </c>
-      <c r="D29">
-        <v>297.5335833</v>
-      </c>
-      <c r="E29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="1">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>792.55536099999995</v>
+      </c>
+      <c r="C36">
+        <v>5.1741333330000003</v>
+      </c>
+      <c r="D36">
+        <v>277.60367500000001</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
         <v>35</v>
       </c>
-      <c r="G29" t="s">
-        <v>52</v>
-      </c>
-      <c r="H29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="1">
-        <v>28</v>
-      </c>
-      <c r="B30">
-        <v>863.5729771</v>
-      </c>
-      <c r="C30">
-        <v>6.415366667</v>
-      </c>
-      <c r="D30">
-        <v>300.3485893</v>
-      </c>
-      <c r="E30" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" t="s">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="1">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>792.55476839999994</v>
+      </c>
+      <c r="C37">
+        <v>5.1741333330000003</v>
+      </c>
+      <c r="D37">
+        <v>277.56829549999998</v>
+      </c>
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" t="s">
         <v>35</v>
       </c>
-      <c r="G30" t="s">
-        <v>52</v>
-      </c>
-      <c r="H30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="1">
-        <v>29</v>
-      </c>
-      <c r="B31">
-        <v>852.5517245</v>
-      </c>
-      <c r="C31">
-        <v>3.467233333</v>
-      </c>
-      <c r="D31">
-        <v>290.3831217</v>
-      </c>
-      <c r="E31" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" t="s">
-        <v>36</v>
-      </c>
-      <c r="G31" t="s">
-        <v>53</v>
-      </c>
-      <c r="H31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="1">
-        <v>30</v>
-      </c>
-      <c r="B32">
-        <v>852.4876705</v>
-      </c>
-      <c r="C32">
-        <v>3.467233333</v>
-      </c>
-      <c r="D32">
-        <v>284.6111068</v>
-      </c>
-      <c r="E32" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" t="s">
-        <v>37</v>
-      </c>
-      <c r="G32" t="s">
-        <v>54</v>
-      </c>
-      <c r="H32" t="s">
-        <v>60</v>
-      </c>
-      <c r="I32" t="s">
-        <v>64</v>
-      </c>
-      <c r="J32" t="s">
-        <v>68</v>
-      </c>
-      <c r="K32" t="s">
-        <v>70</v>
-      </c>
-      <c r="L32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:34">
-      <c r="A33" s="1">
-        <v>31</v>
-      </c>
-      <c r="B33">
-        <v>850.561693</v>
-      </c>
-      <c r="C33">
-        <v>0.897416667</v>
-      </c>
-      <c r="D33">
-        <v>291.8683606</v>
-      </c>
-      <c r="E33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G33" t="s">
-        <v>38</v>
-      </c>
-      <c r="H33" t="s">
-        <v>38</v>
-      </c>
-      <c r="I33" t="s">
-        <v>38</v>
-      </c>
-      <c r="J33" t="s">
-        <v>69</v>
-      </c>
-      <c r="K33" t="s">
-        <v>38</v>
-      </c>
-      <c r="L33" t="s">
-        <v>38</v>
-      </c>
-      <c r="M33" t="s">
-        <v>38</v>
-      </c>
-      <c r="N33" t="s">
-        <v>72</v>
-      </c>
-      <c r="O33" t="s">
-        <v>38</v>
-      </c>
-      <c r="P33" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>38</v>
-      </c>
-      <c r="R33" t="s">
-        <v>38</v>
-      </c>
-      <c r="S33" t="s">
-        <v>38</v>
-      </c>
-      <c r="T33" t="s">
-        <v>38</v>
-      </c>
-      <c r="U33" t="s">
-        <v>38</v>
-      </c>
-      <c r="V33" t="s">
-        <v>38</v>
-      </c>
-      <c r="W33" t="s">
-        <v>38</v>
-      </c>
-      <c r="X33" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z33" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC33" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD33" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE33" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF33" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG33" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:34">
-      <c r="A34" s="1">
-        <v>32</v>
-      </c>
-      <c r="B34">
-        <v>850.5612583</v>
-      </c>
-      <c r="C34">
-        <v>0.897416667</v>
-      </c>
-      <c r="D34">
-        <v>291.8359443</v>
-      </c>
-      <c r="E34" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" t="s">
-        <v>38</v>
-      </c>
-      <c r="G34" t="s">
-        <v>38</v>
-      </c>
-      <c r="H34" t="s">
-        <v>38</v>
-      </c>
-      <c r="I34" t="s">
-        <v>38</v>
-      </c>
-      <c r="J34" t="s">
-        <v>69</v>
-      </c>
-      <c r="K34" t="s">
-        <v>38</v>
-      </c>
-      <c r="L34" t="s">
-        <v>38</v>
-      </c>
-      <c r="M34" t="s">
-        <v>38</v>
-      </c>
-      <c r="N34" t="s">
-        <v>72</v>
-      </c>
-      <c r="O34" t="s">
-        <v>38</v>
-      </c>
-      <c r="P34" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>38</v>
-      </c>
-      <c r="R34" t="s">
-        <v>38</v>
-      </c>
-      <c r="S34" t="s">
-        <v>38</v>
-      </c>
-      <c r="T34" t="s">
-        <v>38</v>
-      </c>
-      <c r="U34" t="s">
-        <v>38</v>
-      </c>
-      <c r="V34" t="s">
-        <v>38</v>
-      </c>
-      <c r="W34" t="s">
-        <v>38</v>
-      </c>
-      <c r="X34" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z34" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA34" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB34" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC34" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD34" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE34" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF34" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG34" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH34" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:34">
-      <c r="A35" s="1">
-        <v>33</v>
-      </c>
-      <c r="B35">
-        <v>828.570821</v>
-      </c>
-      <c r="C35">
-        <v>0.897416667</v>
-      </c>
-      <c r="D35">
-        <v>283.2464333</v>
-      </c>
-      <c r="E35" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" t="s">
-        <v>39</v>
-      </c>
-      <c r="G35" t="s">
-        <v>39</v>
-      </c>
-      <c r="H35" t="s">
-        <v>39</v>
-      </c>
-      <c r="I35" t="s">
-        <v>65</v>
-      </c>
-      <c r="J35" t="s">
-        <v>39</v>
-      </c>
-      <c r="K35" t="s">
-        <v>39</v>
-      </c>
-      <c r="L35" t="s">
-        <v>39</v>
-      </c>
-      <c r="M35" t="s">
-        <v>39</v>
-      </c>
-      <c r="N35" t="s">
-        <v>73</v>
-      </c>
-      <c r="O35" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:34">
-      <c r="A36" s="1">
-        <v>34</v>
-      </c>
-      <c r="B36">
-        <v>828.5707407</v>
-      </c>
-      <c r="C36">
-        <v>0.897416667</v>
-      </c>
-      <c r="D36">
-        <v>283.2795467</v>
-      </c>
-      <c r="E36" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" t="s">
-        <v>39</v>
-      </c>
-      <c r="G36" t="s">
-        <v>39</v>
-      </c>
-      <c r="H36" t="s">
-        <v>39</v>
-      </c>
-      <c r="I36" t="s">
-        <v>65</v>
-      </c>
-      <c r="J36" t="s">
-        <v>39</v>
-      </c>
-      <c r="K36" t="s">
-        <v>39</v>
-      </c>
-      <c r="L36" t="s">
-        <v>39</v>
-      </c>
-      <c r="M36" t="s">
-        <v>39</v>
-      </c>
-      <c r="N36" t="s">
-        <v>73</v>
-      </c>
-      <c r="O36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:34">
-      <c r="A37" s="1">
-        <v>35</v>
-      </c>
-      <c r="B37">
-        <v>797.5450976</v>
-      </c>
-      <c r="C37">
-        <v>1.707</v>
-      </c>
-      <c r="D37">
-        <v>279.0507536</v>
-      </c>
-      <c r="E37" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:34">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B38">
-        <v>797.529183</v>
+        <v>766.53962039999999</v>
       </c>
       <c r="C38">
-        <v>1.707</v>
+        <v>5.1741333330000003</v>
       </c>
       <c r="D38">
-        <v>279.01571</v>
+        <v>271.81468009999998</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
       </c>
       <c r="F38" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:34">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B39">
-        <v>794.570152</v>
+        <v>766.53929289999996</v>
       </c>
       <c r="C39">
-        <v>5.174133333</v>
+        <v>5.1741333330000003</v>
       </c>
       <c r="D39">
-        <v>280.5053798</v>
+        <v>271.77771280000002</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
       </c>
       <c r="F39" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:34">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B40">
-        <v>794.5697036</v>
+        <v>750.54350609999995</v>
       </c>
       <c r="C40">
-        <v>5.174133333</v>
+        <v>5.0528333329999997</v>
       </c>
       <c r="D40">
-        <v>279.0682617</v>
+        <v>270.3798673</v>
       </c>
       <c r="E40" t="s">
         <v>15</v>
       </c>
       <c r="F40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:34">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B41">
-        <v>792.5553609999999</v>
+        <v>750.54242020000004</v>
       </c>
       <c r="C41">
-        <v>5.174133333</v>
+        <v>5.0528333329999997</v>
       </c>
       <c r="D41">
-        <v>277.603675</v>
+        <v>270.41819270000002</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
       </c>
       <c r="F41" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" spans="1:34">
-      <c r="A42" s="1">
-        <v>40</v>
-      </c>
-      <c r="B42">
-        <v>792.5547683999999</v>
-      </c>
-      <c r="C42">
-        <v>5.174133333</v>
-      </c>
-      <c r="D42">
-        <v>277.5682955</v>
-      </c>
-      <c r="E42" t="s">
-        <v>15</v>
-      </c>
-      <c r="F42" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:34">
-      <c r="A43" s="1">
-        <v>41</v>
-      </c>
-      <c r="B43">
-        <v>766.5396204</v>
-      </c>
-      <c r="C43">
-        <v>5.174133333</v>
-      </c>
-      <c r="D43">
-        <v>271.8146801</v>
-      </c>
-      <c r="E43" t="s">
-        <v>15</v>
-      </c>
-      <c r="F43" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="1:34">
-      <c r="A44" s="1">
-        <v>42</v>
-      </c>
-      <c r="B44">
-        <v>766.5392929</v>
-      </c>
-      <c r="C44">
-        <v>5.174133333</v>
-      </c>
-      <c r="D44">
-        <v>271.7777128</v>
-      </c>
-      <c r="E44" t="s">
-        <v>15</v>
-      </c>
-      <c r="F44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:34">
-      <c r="A45" s="1">
-        <v>43</v>
-      </c>
-      <c r="B45">
-        <v>750.5435060999999</v>
-      </c>
-      <c r="C45">
-        <v>5.052833333</v>
-      </c>
-      <c r="D45">
-        <v>270.3798673</v>
-      </c>
-      <c r="E45" t="s">
-        <v>15</v>
-      </c>
-      <c r="F45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:34">
-      <c r="A46" s="1">
-        <v>44</v>
-      </c>
-      <c r="B46">
-        <v>750.5424202</v>
-      </c>
-      <c r="C46">
-        <v>5.052833333</v>
-      </c>
-      <c r="D46">
-        <v>270.4181927</v>
-      </c>
-      <c r="E46" t="s">
-        <v>15</v>
-      </c>
-      <c r="F46" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>